<commit_message>
World evolution according to genes (needs work)
</commit_message>
<xml_diff>
--- a/data/CreatureTypes.xlsx
+++ b/data/CreatureTypes.xlsx
@@ -24,12 +24,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Breeders</t>
+  </si>
+  <si>
+    <t>Hunters</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,8 +60,15 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,6 +96,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -113,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -131,6 +157,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -413,17 +460,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF28"/>
+  <dimension ref="A1:AR28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:O6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="32" width="5.7109375" style="1" customWidth="1"/>
-    <col min="33" max="16384" width="9.140625" style="1"/>
+    <col min="33" max="33" width="9.140625" style="8"/>
+    <col min="34" max="34" width="9.140625" style="11"/>
+    <col min="35" max="44" width="9.140625" style="8"/>
+    <col min="45" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -519,23 +571,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="7">
         <v>2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="7">
         <v>3</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="7">
         <v>4</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="7">
         <v>5</v>
       </c>
       <c r="G2" s="4">
@@ -574,7 +626,7 @@
       <c r="R2" s="4">
         <v>17</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="7">
         <v>18</v>
       </c>
       <c r="T2" s="4">
@@ -617,7 +669,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -714,8 +766,11 @@
       <c r="AF3" s="4">
         <v>62</v>
       </c>
+      <c r="AH3" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -812,8 +867,11 @@
       <c r="AF4" s="4">
         <v>93</v>
       </c>
+      <c r="AH4" s="10" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -832,7 +890,7 @@
       <c r="F5" s="4">
         <v>98</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="7">
         <v>99</v>
       </c>
       <c r="H5" s="4">
@@ -911,7 +969,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -945,16 +1003,16 @@
       <c r="K6" s="4">
         <v>134</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="7">
         <v>135</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="7">
         <v>136</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="7">
         <v>137</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="7">
         <v>138</v>
       </c>
       <c r="P6" s="4">
@@ -1009,7 +1067,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="7" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1107,7 +1165,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1205,95 +1263,95 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="4">
         <v>218</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>219</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="5">
         <v>220</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="5">
         <v>221</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>222</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="13">
         <v>223</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="13">
         <v>224</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="13">
         <v>225</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="13">
         <v>226</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="13">
         <v>227</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="13">
         <v>228</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="13">
         <v>229</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="13">
         <v>230</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="13">
         <v>231</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="13">
         <v>232</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="13">
         <v>233</v>
       </c>
-      <c r="R9" s="5">
+      <c r="R9" s="13">
         <v>234</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="13">
         <v>235</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T9" s="13">
         <v>236</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="13">
         <v>237</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="13">
         <v>238</v>
       </c>
-      <c r="W9" s="4">
+      <c r="W9" s="13">
         <v>239</v>
       </c>
-      <c r="X9" s="4">
+      <c r="X9" s="13">
         <v>240</v>
       </c>
-      <c r="Y9" s="4">
+      <c r="Y9" s="13">
         <v>241</v>
       </c>
-      <c r="Z9" s="4">
+      <c r="Z9" s="13">
         <v>242</v>
       </c>
-      <c r="AA9" s="4">
+      <c r="AA9" s="13">
         <v>243</v>
       </c>
-      <c r="AB9" s="4">
+      <c r="AB9" s="13">
         <v>244</v>
       </c>
-      <c r="AC9" s="4">
+      <c r="AC9" s="13">
         <v>245</v>
       </c>
-      <c r="AD9" s="4">
+      <c r="AD9" s="13">
         <v>246</v>
       </c>
       <c r="AE9" s="4">
@@ -1303,7 +1361,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1322,76 +1380,76 @@
       <c r="F10" s="6">
         <v>253</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="12">
         <v>254</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="12">
         <v>255</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="12">
         <v>256</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="12">
         <v>257</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="12">
         <v>258</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="12">
         <v>259</v>
       </c>
-      <c r="M10" s="6">
+      <c r="M10" s="12">
         <v>260</v>
       </c>
-      <c r="N10" s="6">
+      <c r="N10" s="12">
         <v>261</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="12">
         <v>262</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="12">
         <v>263</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="12">
         <v>264</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="12">
         <v>265</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="12">
         <v>266</v>
       </c>
-      <c r="T10" s="6">
+      <c r="T10" s="12">
         <v>267</v>
       </c>
-      <c r="U10" s="6">
+      <c r="U10" s="12">
         <v>268</v>
       </c>
-      <c r="V10" s="6">
+      <c r="V10" s="12">
         <v>269</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10" s="12">
         <v>270</v>
       </c>
-      <c r="X10" s="6">
+      <c r="X10" s="12">
         <v>271</v>
       </c>
-      <c r="Y10" s="6">
+      <c r="Y10" s="12">
         <v>272</v>
       </c>
-      <c r="Z10" s="6">
+      <c r="Z10" s="12">
         <v>273</v>
       </c>
-      <c r="AA10" s="6">
+      <c r="AA10" s="12">
         <v>274</v>
       </c>
-      <c r="AB10" s="6">
+      <c r="AB10" s="12">
         <v>275</v>
       </c>
-      <c r="AC10" s="6">
+      <c r="AC10" s="12">
         <v>276</v>
       </c>
-      <c r="AD10" s="6">
+      <c r="AD10" s="12">
         <v>277</v>
       </c>
       <c r="AE10" s="4">
@@ -1401,7 +1459,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1499,7 +1557,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1597,7 +1655,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1695,7 +1753,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="14" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1793,7 +1851,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="15" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1848,7 +1906,7 @@
       <c r="R15" s="4">
         <v>420</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S15" s="7">
         <v>421</v>
       </c>
       <c r="T15" s="4">
@@ -1891,7 +1949,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="16" spans="1:32" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -2935,7 +2993,7 @@
       <c r="U26" s="4">
         <v>764</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V26" s="7">
         <v>765</v>
       </c>
       <c r="W26" s="4">

</xml_diff>